<commit_message>
finish module1: product, module2: macro
</commit_message>
<xml_diff>
--- a/auto/new_data/5_經濟數據_china.xlsx
+++ b/auto/new_data/5_經濟數據_china.xlsx
@@ -488,12 +488,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>7.19</t>
+          <t>7.25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.24</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -518,12 +518,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3452</t>
+          <t>3425</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3471</t>
+          <t>3439</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
@@ -2206,12 +2206,12 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
           <t>0.1</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>0.3</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
@@ -2223,7 +2223,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Sep/24</t>
+          <t>Oct/24</t>
         </is>
       </c>
     </row>
@@ -2444,12 +2444,12 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
           <t>-0.1</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>-0.2</t>
         </is>
       </c>
       <c r="E60" t="inlineStr"/>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Sep/24</t>
+          <t>Oct/24</t>
         </is>
       </c>
     </row>
@@ -2478,7 +2478,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>-0.7</t>
+          <t>-0.1</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2495,7 +2495,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Sep/24</t>
+          <t>Oct/24</t>
         </is>
       </c>
     </row>
@@ -2512,12 +2512,12 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
+          <t>-0.3</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
           <t>-0.1</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>-0.3</t>
         </is>
       </c>
       <c r="E62" t="inlineStr"/>
@@ -2529,7 +2529,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Sep/24</t>
+          <t>Oct/24</t>
         </is>
       </c>
     </row>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>1.87</t>
+          <t>1.86</t>
         </is>
       </c>
       <c r="E65" t="inlineStr"/>
@@ -2750,12 +2750,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
           <t>1590</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>900</t>
         </is>
       </c>
       <c r="E69" t="inlineStr"/>
@@ -2767,7 +2767,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Sep/24</t>
+          <t>Oct/24</t>
         </is>
       </c>
     </row>
@@ -2852,12 +2852,12 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
+          <t>14000</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
           <t>37600</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>30300</t>
         </is>
       </c>
       <c r="E72" t="inlineStr"/>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Sep/24</t>
+          <t>Oct/24</t>
         </is>
       </c>
     </row>
@@ -2886,12 +2886,12 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
+          <t>7.8</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
           <t>8.1</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>8.5</t>
         </is>
       </c>
       <c r="E73" t="inlineStr"/>
@@ -2903,7 +2903,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Sep/24</t>
+          <t>Oct/24</t>
         </is>
       </c>
     </row>
@@ -3090,12 +3090,12 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>12.2</t>
+          <t>233</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>19.2</t>
+          <t>126</t>
         </is>
       </c>
       <c r="E79" t="inlineStr"/>
@@ -3464,12 +3464,12 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
+          <t>641</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
           <t>580</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>499</t>
         </is>
       </c>
       <c r="E90" t="inlineStr"/>
@@ -3481,7 +3481,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Aug/24</t>
+          <t>Sep/24</t>
         </is>
       </c>
     </row>
@@ -3566,12 +3566,12 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
+          <t>4215</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
           <t>4250</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>4274</t>
         </is>
       </c>
       <c r="E93" t="inlineStr"/>
@@ -3579,7 +3579,7 @@
       <c r="G93" t="inlineStr"/>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Jun/24</t>
+          <t>Jul/24</t>
         </is>
       </c>
     </row>
@@ -4234,12 +4234,12 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
+          <t>1258</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
           <t>12113</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>19750</t>
         </is>
       </c>
       <c r="E113" t="inlineStr"/>
@@ -4251,7 +4251,7 @@
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Aug/24</t>
+          <t>Sep/24</t>
         </is>
       </c>
     </row>
@@ -4268,12 +4268,12 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
+          <t>2788</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
           <t>18435</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>18892</t>
         </is>
       </c>
       <c r="E114" t="inlineStr"/>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Aug/24</t>
+          <t>Sep/24</t>
         </is>
       </c>
     </row>
@@ -4800,12 +4800,12 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
+          <t>3050000</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
           <t>2809000</t>
-        </is>
-      </c>
-      <c r="D130" t="inlineStr">
-        <is>
-          <t>2453000</t>
         </is>
       </c>
       <c r="E130" t="inlineStr"/>
@@ -4817,7 +4817,7 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>Sep/24</t>
+          <t>Oct/24</t>
         </is>
       </c>
     </row>
@@ -4834,7 +4834,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>149</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -4851,7 +4851,7 @@
       </c>
       <c r="H131" t="inlineStr">
         <is>
-          <t>Aug/24</t>
+          <t>Sep/24</t>
         </is>
       </c>
     </row>

</xml_diff>